<commit_message>
No of iteration added in Config file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UIPath\POC\POC-Dispatcher_Performer_Model\POC-Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{957A25A0-9E91-4251-B6B9-657A5BFC8EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1649EA26-0F0E-4863-B32F-C1AF136261ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="2160" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>https://careers.persistent.com/referral/#/job-list</t>
+  </si>
+  <si>
+    <t>ItemsNo</t>
   </si>
 </sst>
 </file>
@@ -550,7 +553,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -646,7 +649,14 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>